<commit_message>
modify: modify new all data
</commit_message>
<xml_diff>
--- a/ALL/ALL_data_grouped_processed_des.xlsx
+++ b/ALL/ALL_data_grouped_processed_des.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Dmax(mm)</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Ru</t>
+  </si>
+  <si>
+    <t>Be</t>
+  </si>
+  <si>
+    <t>Rh</t>
   </si>
   <si>
     <t>count</t>
@@ -563,13 +569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE9"/>
+  <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:59">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,529 +744,553 @@
       <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="BF1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:57">
+    <row r="2" spans="1:59">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2">
-        <v>795</v>
+        <v>834</v>
       </c>
       <c r="C2">
-        <v>829</v>
+        <v>906</v>
       </c>
       <c r="D2">
-        <v>769</v>
+        <v>845</v>
       </c>
       <c r="E2">
-        <v>785</v>
+        <v>834</v>
       </c>
       <c r="F2">
-        <v>89</v>
+        <v>404</v>
       </c>
       <c r="G2">
-        <v>280</v>
+        <v>411</v>
       </c>
       <c r="H2">
+        <v>349</v>
+      </c>
+      <c r="I2">
+        <v>1390</v>
+      </c>
+      <c r="J2">
+        <v>1390</v>
+      </c>
+      <c r="K2">
+        <v>1390</v>
+      </c>
+      <c r="L2">
+        <v>1390</v>
+      </c>
+      <c r="M2">
+        <v>1390</v>
+      </c>
+      <c r="N2">
+        <v>1390</v>
+      </c>
+      <c r="O2">
+        <v>1390</v>
+      </c>
+      <c r="P2">
+        <v>1390</v>
+      </c>
+      <c r="Q2">
+        <v>1390</v>
+      </c>
+      <c r="R2">
+        <v>1390</v>
+      </c>
+      <c r="S2">
+        <v>1390</v>
+      </c>
+      <c r="T2">
+        <v>1390</v>
+      </c>
+      <c r="U2">
+        <v>1390</v>
+      </c>
+      <c r="V2">
+        <v>1390</v>
+      </c>
+      <c r="W2">
+        <v>1390</v>
+      </c>
+      <c r="X2">
+        <v>1390</v>
+      </c>
+      <c r="Y2">
+        <v>1390</v>
+      </c>
+      <c r="Z2">
+        <v>1390</v>
+      </c>
+      <c r="AA2">
+        <v>1390</v>
+      </c>
+      <c r="AB2">
+        <v>1390</v>
+      </c>
+      <c r="AC2">
+        <v>1390</v>
+      </c>
+      <c r="AD2">
+        <v>1390</v>
+      </c>
+      <c r="AE2">
+        <v>1390</v>
+      </c>
+      <c r="AF2">
+        <v>1390</v>
+      </c>
+      <c r="AG2">
+        <v>1390</v>
+      </c>
+      <c r="AH2">
+        <v>1390</v>
+      </c>
+      <c r="AI2">
+        <v>1390</v>
+      </c>
+      <c r="AJ2">
+        <v>1390</v>
+      </c>
+      <c r="AK2">
+        <v>1390</v>
+      </c>
+      <c r="AL2">
+        <v>1390</v>
+      </c>
+      <c r="AM2">
+        <v>1390</v>
+      </c>
+      <c r="AN2">
+        <v>1390</v>
+      </c>
+      <c r="AO2">
+        <v>1390</v>
+      </c>
+      <c r="AP2">
+        <v>1390</v>
+      </c>
+      <c r="AQ2">
+        <v>1390</v>
+      </c>
+      <c r="AR2">
+        <v>1390</v>
+      </c>
+      <c r="AS2">
+        <v>1390</v>
+      </c>
+      <c r="AT2">
+        <v>1390</v>
+      </c>
+      <c r="AU2">
+        <v>1390</v>
+      </c>
+      <c r="AV2">
+        <v>1390</v>
+      </c>
+      <c r="AW2">
+        <v>1390</v>
+      </c>
+      <c r="AX2">
+        <v>1390</v>
+      </c>
+      <c r="AY2">
+        <v>1390</v>
+      </c>
+      <c r="AZ2">
+        <v>1390</v>
+      </c>
+      <c r="BA2">
+        <v>1390</v>
+      </c>
+      <c r="BB2">
+        <v>1390</v>
+      </c>
+      <c r="BC2">
+        <v>1390</v>
+      </c>
+      <c r="BD2">
+        <v>1390</v>
+      </c>
+      <c r="BE2">
+        <v>1390</v>
+      </c>
+      <c r="BF2">
+        <v>1390</v>
+      </c>
+      <c r="BG2">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I2">
-        <v>1019</v>
-      </c>
-      <c r="J2">
-        <v>1019</v>
-      </c>
-      <c r="K2">
-        <v>1019</v>
-      </c>
-      <c r="L2">
-        <v>1019</v>
-      </c>
-      <c r="M2">
-        <v>1019</v>
-      </c>
-      <c r="N2">
-        <v>1019</v>
-      </c>
-      <c r="O2">
-        <v>1019</v>
-      </c>
-      <c r="P2">
-        <v>1019</v>
-      </c>
-      <c r="Q2">
-        <v>1019</v>
-      </c>
-      <c r="R2">
-        <v>1019</v>
-      </c>
-      <c r="S2">
-        <v>1019</v>
-      </c>
-      <c r="T2">
-        <v>1019</v>
-      </c>
-      <c r="U2">
-        <v>1019</v>
-      </c>
-      <c r="V2">
-        <v>1019</v>
-      </c>
-      <c r="W2">
-        <v>1019</v>
-      </c>
-      <c r="X2">
-        <v>1019</v>
-      </c>
-      <c r="Y2">
-        <v>1019</v>
-      </c>
-      <c r="Z2">
-        <v>1019</v>
-      </c>
-      <c r="AA2">
-        <v>1019</v>
-      </c>
-      <c r="AB2">
-        <v>1019</v>
-      </c>
-      <c r="AC2">
-        <v>1019</v>
-      </c>
-      <c r="AD2">
-        <v>1019</v>
-      </c>
-      <c r="AE2">
-        <v>1019</v>
-      </c>
-      <c r="AF2">
-        <v>1019</v>
-      </c>
-      <c r="AG2">
-        <v>1019</v>
-      </c>
-      <c r="AH2">
-        <v>1019</v>
-      </c>
-      <c r="AI2">
-        <v>1019</v>
-      </c>
-      <c r="AJ2">
-        <v>1019</v>
-      </c>
-      <c r="AK2">
-        <v>1019</v>
-      </c>
-      <c r="AL2">
-        <v>1019</v>
-      </c>
-      <c r="AM2">
-        <v>1019</v>
-      </c>
-      <c r="AN2">
-        <v>1019</v>
-      </c>
-      <c r="AO2">
-        <v>1019</v>
-      </c>
-      <c r="AP2">
-        <v>1019</v>
-      </c>
-      <c r="AQ2">
-        <v>1019</v>
-      </c>
-      <c r="AR2">
-        <v>1019</v>
-      </c>
-      <c r="AS2">
-        <v>1019</v>
-      </c>
-      <c r="AT2">
-        <v>1019</v>
-      </c>
-      <c r="AU2">
-        <v>1019</v>
-      </c>
-      <c r="AV2">
-        <v>1019</v>
-      </c>
-      <c r="AW2">
-        <v>1019</v>
-      </c>
-      <c r="AX2">
-        <v>1019</v>
-      </c>
-      <c r="AY2">
-        <v>1019</v>
-      </c>
-      <c r="AZ2">
-        <v>1019</v>
-      </c>
-      <c r="BA2">
-        <v>1019</v>
-      </c>
-      <c r="BB2">
-        <v>1019</v>
-      </c>
-      <c r="BC2">
-        <v>1019</v>
-      </c>
-      <c r="BD2">
-        <v>1019</v>
-      </c>
-      <c r="BE2">
-        <v>1019</v>
+      <c r="B3">
+        <v>5.453333333333333</v>
+      </c>
+      <c r="C3">
+        <v>627.1862141280353</v>
+      </c>
+      <c r="D3">
+        <v>678.6912130177515</v>
+      </c>
+      <c r="E3">
+        <v>1077.979978017586</v>
+      </c>
+      <c r="F3">
+        <v>1498.894801980198</v>
+      </c>
+      <c r="G3">
+        <v>95.21029115977291</v>
+      </c>
+      <c r="H3">
+        <v>11.23491404011461</v>
+      </c>
+      <c r="I3">
+        <v>7.953378006139089</v>
+      </c>
+      <c r="J3">
+        <v>2.262707243597122</v>
+      </c>
+      <c r="K3">
+        <v>2.753222005827338</v>
+      </c>
+      <c r="L3">
+        <v>0.8191539568345324</v>
+      </c>
+      <c r="M3">
+        <v>1.797829568345324</v>
+      </c>
+      <c r="N3">
+        <v>0.7275246121582734</v>
+      </c>
+      <c r="O3">
+        <v>9.979172850935251</v>
+      </c>
+      <c r="P3">
+        <v>0.664306324028777</v>
+      </c>
+      <c r="Q3">
+        <v>1.723711329784173</v>
+      </c>
+      <c r="R3">
+        <v>0.7536710272661871</v>
+      </c>
+      <c r="S3">
+        <v>3.67751593266187</v>
+      </c>
+      <c r="T3">
+        <v>0.373884892086331</v>
+      </c>
+      <c r="U3">
+        <v>0.03097841726618705</v>
+      </c>
+      <c r="V3">
+        <v>1.887338129496403</v>
+      </c>
+      <c r="W3">
+        <v>14.19096254191847</v>
+      </c>
+      <c r="X3">
+        <v>15.96128125151079</v>
+      </c>
+      <c r="Y3">
+        <v>4.408361108776978</v>
+      </c>
+      <c r="Z3">
+        <v>6.304569730863308</v>
+      </c>
+      <c r="AA3">
+        <v>5.370604316546762</v>
+      </c>
+      <c r="AB3">
+        <v>1.53136690647482</v>
+      </c>
+      <c r="AC3">
+        <v>0.6839568345323741</v>
+      </c>
+      <c r="AD3">
+        <v>3.237122302158274</v>
+      </c>
+      <c r="AE3">
+        <v>0.03884892086330935</v>
+      </c>
+      <c r="AF3">
+        <v>1.286968244316547</v>
+      </c>
+      <c r="AG3">
+        <v>0.1137122302158273</v>
+      </c>
+      <c r="AH3">
+        <v>0.006474820143884892</v>
+      </c>
+      <c r="AI3">
+        <v>3.447913669064748</v>
+      </c>
+      <c r="AJ3">
+        <v>0.5503597122302158</v>
+      </c>
+      <c r="AK3">
+        <v>0.3364748201438849</v>
+      </c>
+      <c r="AL3">
+        <v>0.146205035971223</v>
+      </c>
+      <c r="AM3">
+        <v>0.1460431654676259</v>
+      </c>
+      <c r="AN3">
+        <v>0.8902877697841727</v>
+      </c>
+      <c r="AO3">
+        <v>0.1503597122302158</v>
+      </c>
+      <c r="AP3">
+        <v>1.881798561151079</v>
+      </c>
+      <c r="AQ3">
+        <v>0.1330935251798561</v>
+      </c>
+      <c r="AR3">
+        <v>0.963402131438849</v>
+      </c>
+      <c r="AS3">
+        <v>0.2056951320863309</v>
+      </c>
+      <c r="AT3">
+        <v>0.1782610719424461</v>
+      </c>
+      <c r="AU3">
+        <v>0.2497841726618705</v>
+      </c>
+      <c r="AV3">
+        <v>1.108250782661871</v>
+      </c>
+      <c r="AW3">
+        <v>0.3415162313669065</v>
+      </c>
+      <c r="AX3">
+        <v>0.092</v>
+      </c>
+      <c r="AY3">
+        <v>0.06676978417266187</v>
+      </c>
+      <c r="AZ3">
+        <v>0.0683453237410072</v>
+      </c>
+      <c r="BA3">
+        <v>0.1</v>
+      </c>
+      <c r="BB3">
+        <v>0.1010791366906475</v>
+      </c>
+      <c r="BC3">
+        <v>0.001438848920863309</v>
+      </c>
+      <c r="BD3">
+        <v>0.223021582733813</v>
+      </c>
+      <c r="BE3">
+        <v>0.07913669064748201</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:57">
-      <c r="A3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3">
-        <v>5.391295597484277</v>
-      </c>
-      <c r="C3">
-        <v>622.4375271411338</v>
-      </c>
-      <c r="D3">
-        <v>672.2621261378414</v>
-      </c>
-      <c r="E3">
-        <v>1072.610702760085</v>
-      </c>
-      <c r="F3">
-        <v>1810.52808988764</v>
-      </c>
-      <c r="G3">
-        <v>90.3387023809524</v>
-      </c>
-      <c r="H3">
-        <v>3.747372881355932</v>
-      </c>
-      <c r="I3">
-        <v>7.406217500817795</v>
-      </c>
-      <c r="J3">
-        <v>0.4641069676153091</v>
-      </c>
-      <c r="K3">
-        <v>1.003395485770363</v>
-      </c>
-      <c r="L3">
-        <v>1.117393523061825</v>
-      </c>
-      <c r="M3">
-        <v>2.452387733071639</v>
-      </c>
-      <c r="N3">
-        <v>0.7695040824337587</v>
-      </c>
-      <c r="O3">
-        <v>10.87181261040236</v>
-      </c>
-      <c r="P3">
-        <v>0.8304816486751717</v>
-      </c>
-      <c r="Q3">
-        <v>0.8067203140333661</v>
-      </c>
-      <c r="R3">
-        <v>0.9880863591756625</v>
-      </c>
-      <c r="S3">
-        <v>2.358638370951914</v>
-      </c>
-      <c r="T3">
-        <v>0.5100098135426889</v>
-      </c>
-      <c r="U3">
-        <v>0.04225711481844946</v>
-      </c>
-      <c r="V3">
-        <v>2.549950932286555</v>
-      </c>
-      <c r="W3">
-        <v>16.11899113509977</v>
-      </c>
-      <c r="X3">
-        <v>15.7166182531894</v>
-      </c>
-      <c r="Y3">
-        <v>2.598561334641806</v>
-      </c>
-      <c r="Z3">
-        <v>5.469131795878312</v>
-      </c>
-      <c r="AA3">
-        <v>7.306319921491659</v>
-      </c>
-      <c r="AB3">
-        <v>1.883120706575073</v>
-      </c>
-      <c r="AC3">
-        <v>0.9329735034347399</v>
-      </c>
-      <c r="AD3">
-        <v>4.415701668302257</v>
-      </c>
-      <c r="AE3">
-        <v>0.05299313052011776</v>
-      </c>
-      <c r="AF3">
-        <v>0.8634936211972521</v>
-      </c>
-      <c r="AG3">
-        <v>0.1354857703631011</v>
-      </c>
-      <c r="AH3">
-        <v>0.008832188420019628</v>
-      </c>
-      <c r="AI3">
-        <v>4.703238469087341</v>
-      </c>
-      <c r="AJ3">
-        <v>0.7311089303238469</v>
-      </c>
-      <c r="AK3">
-        <v>0.4589793915603533</v>
-      </c>
-      <c r="AL3">
-        <v>0.1994357212953876</v>
-      </c>
-      <c r="AM3">
-        <v>0.1992149165848871</v>
-      </c>
-      <c r="AN3">
-        <v>1.214425907752699</v>
-      </c>
-      <c r="AO3">
-        <v>0.2051030421982336</v>
-      </c>
-      <c r="AP3">
-        <v>2.566928361138371</v>
-      </c>
-      <c r="AQ3">
-        <v>0.1717369970559372</v>
-      </c>
-      <c r="AR3">
-        <v>0.1206084396467125</v>
-      </c>
-      <c r="AS3">
-        <v>0.02849067713444553</v>
-      </c>
-      <c r="AT3">
-        <v>0.2431627968596664</v>
-      </c>
-      <c r="AU3">
-        <v>0.3407262021589794</v>
-      </c>
-      <c r="AV3">
-        <v>0.003925417075564278</v>
-      </c>
-      <c r="AW3">
-        <v>0.1609421000981354</v>
-      </c>
-      <c r="AX3">
-        <v>0.12549558390579</v>
-      </c>
-      <c r="AY3">
-        <v>0.07145240431795878</v>
-      </c>
-      <c r="AZ3">
-        <v>0.09322865554465162</v>
-      </c>
-      <c r="BA3">
-        <v>0.1364082433758587</v>
-      </c>
-      <c r="BB3">
-        <v>0.1378802747791953</v>
-      </c>
-      <c r="BC3">
-        <v>0.001962708537782139</v>
-      </c>
-      <c r="BD3">
-        <v>0.3042198233562316</v>
-      </c>
-      <c r="BE3">
-        <v>0.1079489695780177</v>
+    <row r="4" spans="1:59">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>5.431903282396297</v>
+      </c>
+      <c r="C4">
+        <v>169.1877493939813</v>
+      </c>
+      <c r="D4">
+        <v>173.6986351574478</v>
+      </c>
+      <c r="E4">
+        <v>262.58747805027</v>
+      </c>
+      <c r="F4">
+        <v>540.7758774441767</v>
+      </c>
+      <c r="G4">
+        <v>52.16760322197145</v>
+      </c>
+      <c r="H4">
+        <v>13.3406361212285</v>
+      </c>
+      <c r="I4">
+        <v>14.09229099443488</v>
+      </c>
+      <c r="J4">
+        <v>5.998028181486877</v>
+      </c>
+      <c r="K4">
+        <v>7.03014719956617</v>
+      </c>
+      <c r="L4">
+        <v>3.542116910970355</v>
+      </c>
+      <c r="M4">
+        <v>5.473866290229083</v>
+      </c>
+      <c r="N4">
+        <v>2.732375015446707</v>
+      </c>
+      <c r="O4">
+        <v>20.81456603418074</v>
+      </c>
+      <c r="P4">
+        <v>2.859138002571895</v>
+      </c>
+      <c r="Q4">
+        <v>5.237710182681127</v>
+      </c>
+      <c r="R4">
+        <v>3.632715746445505</v>
+      </c>
+      <c r="S4">
+        <v>8.37784974579076</v>
+      </c>
+      <c r="T4">
+        <v>4.868252896536655</v>
+      </c>
+      <c r="U4">
+        <v>0.6375922521670045</v>
+      </c>
+      <c r="V4">
+        <v>10.69904206874055</v>
+      </c>
+      <c r="W4">
+        <v>16.41068038296234</v>
+      </c>
+      <c r="X4">
+        <v>22.92972514475662</v>
+      </c>
+      <c r="Y4">
+        <v>9.291389539472128</v>
+      </c>
+      <c r="Z4">
+        <v>8.036790095396755</v>
+      </c>
+      <c r="AA4">
+        <v>15.92791845294328</v>
+      </c>
+      <c r="AB4">
+        <v>6.220221662084851</v>
+      </c>
+      <c r="AC4">
+        <v>4.821561263189952</v>
+      </c>
+      <c r="AD4">
+        <v>13.32222006680703</v>
+      </c>
+      <c r="AE4">
+        <v>0.4090429912164888</v>
+      </c>
+      <c r="AF4">
+        <v>5.458712152055919</v>
+      </c>
+      <c r="AG4">
+        <v>0.7977552401886467</v>
+      </c>
+      <c r="AH4">
+        <v>0.1952306173886432</v>
+      </c>
+      <c r="AI4">
+        <v>12.83469831687764</v>
+      </c>
+      <c r="AJ4">
+        <v>3.282200487980483</v>
+      </c>
+      <c r="AK4">
+        <v>4.067162988863774</v>
+      </c>
+      <c r="AL4">
+        <v>2.254861336037147</v>
+      </c>
+      <c r="AM4">
+        <v>2.263644054215008</v>
+      </c>
+      <c r="AN4">
+        <v>7.34182956763585</v>
+      </c>
+      <c r="AO4">
+        <v>2.450308868167382</v>
+      </c>
+      <c r="AP4">
+        <v>10.64328034438949</v>
+      </c>
+      <c r="AQ4">
+        <v>2.053352050203425</v>
+      </c>
+      <c r="AR4">
+        <v>4.288062978649821</v>
+      </c>
+      <c r="AS4">
+        <v>1.807073019743419</v>
+      </c>
+      <c r="AT4">
+        <v>2.74732711424564</v>
+      </c>
+      <c r="AU4">
+        <v>3.795730515693905</v>
+      </c>
+      <c r="AV4">
+        <v>4.692894163695687</v>
+      </c>
+      <c r="AW4">
+        <v>3.08089207406406</v>
+      </c>
+      <c r="AX4">
+        <v>1.807563311751408</v>
+      </c>
+      <c r="AY4">
+        <v>0.8968386988673681</v>
+      </c>
+      <c r="AZ4">
+        <v>1.823474478878782</v>
+      </c>
+      <c r="BA4">
+        <v>2.17272509564667</v>
+      </c>
+      <c r="BB4">
+        <v>1.974650069025035</v>
+      </c>
+      <c r="BC4">
+        <v>0.05364417807858241</v>
+      </c>
+      <c r="BD4">
+        <v>3.3545970424223</v>
+      </c>
+      <c r="BE4">
+        <v>1.702345598184398</v>
+      </c>
+      <c r="BF4">
+        <v>0</v>
+      </c>
+      <c r="BG4">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:57">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4">
-        <v>5.388533231298136</v>
-      </c>
-      <c r="C4">
-        <v>175.8345237405331</v>
-      </c>
-      <c r="D4">
-        <v>180.5734840544634</v>
-      </c>
-      <c r="E4">
-        <v>269.5301221173185</v>
-      </c>
-      <c r="F4">
-        <v>467.8775599810382</v>
-      </c>
-      <c r="G4">
-        <v>58.11464247326671</v>
-      </c>
-      <c r="H4">
-        <v>5.392749311290513</v>
-      </c>
-      <c r="I4">
-        <v>15.35021670827524</v>
-      </c>
-      <c r="J4">
-        <v>2.227451484379749</v>
-      </c>
-      <c r="K4">
-        <v>4.154105935268582</v>
-      </c>
-      <c r="L4">
-        <v>4.0970104886614</v>
-      </c>
-      <c r="M4">
-        <v>6.267072705646052</v>
-      </c>
-      <c r="N4">
-        <v>2.7122932474411</v>
-      </c>
-      <c r="O4">
-        <v>23.54776448513113</v>
-      </c>
-      <c r="P4">
-        <v>3.167257282781172</v>
-      </c>
-      <c r="Q4">
-        <v>3.383096465195532</v>
-      </c>
-      <c r="R4">
-        <v>4.16908492647548</v>
-      </c>
-      <c r="S4">
-        <v>7.470936886934254</v>
-      </c>
-      <c r="T4">
-        <v>5.680456093843894</v>
-      </c>
-      <c r="U4">
-        <v>0.7444463724208389</v>
-      </c>
-      <c r="V4">
-        <v>12.42654596792966</v>
-      </c>
-      <c r="W4">
-        <v>16.96563992058172</v>
-      </c>
-      <c r="X4">
-        <v>23.2799795067074</v>
-      </c>
-      <c r="Y4">
-        <v>8.237696019646419</v>
-      </c>
-      <c r="Z4">
-        <v>7.688360569354828</v>
-      </c>
-      <c r="AA4">
-        <v>18.21296939341437</v>
-      </c>
-      <c r="AB4">
-        <v>7.026336582619034</v>
-      </c>
-      <c r="AC4">
-        <v>5.611345867637484</v>
-      </c>
-      <c r="AD4">
-        <v>15.39329625265222</v>
-      </c>
-      <c r="AE4">
-        <v>0.4770142598272044</v>
-      </c>
-      <c r="AF4">
-        <v>5.038342373538544</v>
-      </c>
-      <c r="AG4">
-        <v>0.688986068150699</v>
-      </c>
-      <c r="AH4">
-        <v>0.2280017197058468</v>
-      </c>
-      <c r="AI4">
-        <v>14.79370184424532</v>
-      </c>
-      <c r="AJ4">
-        <v>3.766231909557769</v>
-      </c>
-      <c r="AK4">
-        <v>4.744895441322594</v>
-      </c>
-      <c r="AL4">
-        <v>2.63186856099189</v>
-      </c>
-      <c r="AM4">
-        <v>2.642139874391196</v>
-      </c>
-      <c r="AN4">
-        <v>8.552932259461027</v>
-      </c>
-      <c r="AO4">
-        <v>2.860223359492906</v>
-      </c>
-      <c r="AP4">
-        <v>12.36133363514831</v>
-      </c>
-      <c r="AQ4">
-        <v>2.391238515093366</v>
-      </c>
-      <c r="AR4">
-        <v>1.525689390625578</v>
-      </c>
-      <c r="AS4">
-        <v>0.5003710633546615</v>
-      </c>
-      <c r="AT4">
-        <v>3.206669954366894</v>
-      </c>
-      <c r="AU4">
-        <v>4.430265158416653</v>
-      </c>
-      <c r="AV4">
-        <v>0.08856140318049563</v>
-      </c>
-      <c r="AW4">
-        <v>2.494710611858472</v>
-      </c>
-      <c r="AX4">
-        <v>2.11040448658178</v>
-      </c>
-      <c r="AY4">
-        <v>0.8399378137014867</v>
-      </c>
-      <c r="AZ4">
-        <v>2.129441683590946</v>
-      </c>
-      <c r="BA4">
-        <v>2.536964302560515</v>
-      </c>
-      <c r="BB4">
-        <v>2.305472651486467</v>
-      </c>
-      <c r="BC4">
-        <v>0.06265314896766491</v>
-      </c>
-      <c r="BD4">
-        <v>3.915323261545137</v>
-      </c>
-      <c r="BE4">
-        <v>1.987714134056831</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57">
+    <row r="5" spans="1:59">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5">
         <v>0.06</v>
@@ -1275,7 +1305,7 @@
         <v>581</v>
       </c>
       <c r="F5">
-        <v>919</v>
+        <v>136</v>
       </c>
       <c r="G5">
         <v>16</v>
@@ -1430,31 +1460,37 @@
       <c r="BE5">
         <v>0</v>
       </c>
+      <c r="BF5">
+        <v>0</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:57">
+    <row r="6" spans="1:59">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>424</v>
+        <v>427.25</v>
       </c>
       <c r="D6">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="E6">
-        <v>785</v>
+        <v>798</v>
       </c>
       <c r="F6">
-        <v>1583</v>
+        <v>1208.5</v>
       </c>
       <c r="G6">
-        <v>49.96</v>
+        <v>62.12</v>
       </c>
       <c r="H6">
-        <v>0.46</v>
+        <v>1.9</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1603,31 +1639,37 @@
       <c r="BE6">
         <v>0</v>
       </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:57">
+    <row r="7" spans="1:59">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>668</v>
+        <v>668.3499999999999</v>
       </c>
       <c r="D7">
-        <v>729.8</v>
+        <v>732</v>
       </c>
       <c r="E7">
-        <v>1142</v>
+        <v>1146.5</v>
       </c>
       <c r="F7">
-        <v>1745</v>
+        <v>1516.5</v>
       </c>
       <c r="G7">
-        <v>80</v>
+        <v>88.90000000000001</v>
       </c>
       <c r="H7">
-        <v>1.5</v>
+        <v>5.8</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1672,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>14</v>
+        <v>9.57845</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1776,34 +1818,40 @@
       <c r="BE7">
         <v>0</v>
       </c>
+      <c r="BF7">
+        <v>0</v>
+      </c>
+      <c r="BG7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:57">
+    <row r="8" spans="1:59">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="D8">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="E8">
-        <v>1275</v>
+        <v>1258</v>
       </c>
       <c r="F8">
-        <v>1874</v>
+        <v>1780</v>
       </c>
       <c r="G8">
-        <v>101.125</v>
+        <v>107.3</v>
       </c>
       <c r="H8">
-        <v>5.6</v>
+        <v>15</v>
       </c>
       <c r="I8">
-        <v>9.460000000000001</v>
+        <v>11.133527775</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1821,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>7.4875</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1845,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="X8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z8">
         <v>10</v>
@@ -1949,10 +1997,16 @@
       <c r="BE8">
         <v>0</v>
       </c>
+      <c r="BF8">
+        <v>0</v>
+      </c>
+      <c r="BG8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:57">
+    <row r="9" spans="1:59">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>35</v>
@@ -1973,13 +2027,13 @@
         <v>309</v>
       </c>
       <c r="H9">
-        <v>32.9</v>
+        <v>75</v>
       </c>
       <c r="I9">
         <v>100</v>
       </c>
       <c r="J9">
-        <v>15</v>
+        <v>27.2727273</v>
       </c>
       <c r="K9">
         <v>50</v>
@@ -1997,7 +2051,7 @@
         <v>91</v>
       </c>
       <c r="P9">
-        <v>19</v>
+        <v>23.0769231</v>
       </c>
       <c r="Q9">
         <v>52</v>
@@ -2021,7 +2075,7 @@
         <v>64</v>
       </c>
       <c r="X9">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Y9">
         <v>53</v>
@@ -2048,7 +2102,7 @@
         <v>51</v>
       </c>
       <c r="AG9">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="AH9">
         <v>7</v>
@@ -2084,7 +2138,7 @@
         <v>42</v>
       </c>
       <c r="AS9">
-        <v>11.032</v>
+        <v>20</v>
       </c>
       <c r="AT9">
         <v>55</v>
@@ -2093,7 +2147,7 @@
         <v>74.7</v>
       </c>
       <c r="AV9">
-        <v>2</v>
+        <v>42.8571429</v>
       </c>
       <c r="AW9">
         <v>46</v>
@@ -2102,7 +2156,7 @@
         <v>55</v>
       </c>
       <c r="AY9">
-        <v>14.54</v>
+        <v>20</v>
       </c>
       <c r="AZ9">
         <v>55</v>
@@ -2121,6 +2175,12 @@
       </c>
       <c r="BE9">
         <v>37</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify: modify final data figures
</commit_message>
<xml_diff>
--- a/ALL/ALL_data_grouped_processed_des.xlsx
+++ b/ALL/ALL_data_grouped_processed_des.xlsx
@@ -756,178 +756,178 @@
         <v>58</v>
       </c>
       <c r="B2">
-        <v>834</v>
+        <v>805</v>
       </c>
       <c r="C2">
-        <v>906</v>
+        <v>871</v>
       </c>
       <c r="D2">
-        <v>845</v>
+        <v>812</v>
       </c>
       <c r="E2">
-        <v>834</v>
+        <v>811</v>
       </c>
       <c r="F2">
-        <v>404</v>
+        <v>320</v>
       </c>
       <c r="G2">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="H2">
-        <v>349</v>
+        <v>280</v>
       </c>
       <c r="I2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="J2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="K2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="L2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="M2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="N2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="O2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="P2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="Q2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="R2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="S2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="T2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="U2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="V2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="W2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="X2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="Y2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="Z2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AA2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AB2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AC2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AD2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AE2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AF2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AG2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AH2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AI2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AJ2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AK2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AL2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AM2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AN2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AO2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AP2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AQ2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AR2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AS2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AT2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AU2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AV2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AW2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AX2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AY2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="AZ2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BA2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BB2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BC2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BD2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BE2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BF2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
       <c r="BG2">
-        <v>1390</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="3" spans="1:59">
@@ -935,172 +935,172 @@
         <v>59</v>
       </c>
       <c r="B3">
-        <v>5.453333333333333</v>
+        <v>5.472894409937888</v>
       </c>
       <c r="C3">
-        <v>627.1862141280353</v>
+        <v>625.4120283199388</v>
       </c>
       <c r="D3">
-        <v>678.6912130177515</v>
+        <v>676.4246408045977</v>
       </c>
       <c r="E3">
-        <v>1077.979978017586</v>
+        <v>1075.919340320592</v>
       </c>
       <c r="F3">
-        <v>1498.894801980198</v>
+        <v>1542.71484375</v>
       </c>
       <c r="G3">
-        <v>95.21029115977291</v>
+        <v>94.93711338448422</v>
       </c>
       <c r="H3">
-        <v>11.23491404011461</v>
+        <v>10.80166369047619</v>
       </c>
       <c r="I3">
-        <v>7.953378006139089</v>
+        <v>7.705899159364328</v>
       </c>
       <c r="J3">
-        <v>2.262707243597122</v>
+        <v>1.757968630260047</v>
       </c>
       <c r="K3">
-        <v>2.753222005827338</v>
+        <v>2.531229395744681</v>
       </c>
       <c r="L3">
-        <v>0.8191539568345324</v>
+        <v>0.8972608353033883</v>
       </c>
       <c r="M3">
-        <v>1.797829568345324</v>
+        <v>1.969253821907014</v>
       </c>
       <c r="N3">
-        <v>0.7275246121582734</v>
+        <v>0.7897307342789599</v>
       </c>
       <c r="O3">
-        <v>9.979172850935251</v>
+        <v>10.15173316469661</v>
       </c>
       <c r="P3">
-        <v>0.664306324028777</v>
+        <v>0.7276483769897557</v>
       </c>
       <c r="Q3">
-        <v>1.723711329784173</v>
+        <v>1.721290255476753</v>
       </c>
       <c r="R3">
-        <v>0.7536710272661871</v>
+        <v>0.8200179100866825</v>
       </c>
       <c r="S3">
-        <v>3.67751593266187</v>
+        <v>3.374662150985028</v>
       </c>
       <c r="T3">
-        <v>0.373884892086331</v>
+        <v>0.4095350669818755</v>
       </c>
       <c r="U3">
-        <v>0.03097841726618705</v>
+        <v>0.03393223010244287</v>
       </c>
       <c r="V3">
-        <v>1.887338129496403</v>
+        <v>2.067297084318361</v>
       </c>
       <c r="W3">
-        <v>14.19096254191847</v>
+        <v>14.30319076246388</v>
       </c>
       <c r="X3">
-        <v>15.96128125151079</v>
+        <v>15.55751966485421</v>
       </c>
       <c r="Y3">
-        <v>4.408361108776978</v>
+        <v>4.066851112923562</v>
       </c>
       <c r="Z3">
-        <v>6.304569730863308</v>
+        <v>6.022582594562648</v>
       </c>
       <c r="AA3">
-        <v>5.370604316546762</v>
+        <v>5.882695035460993</v>
       </c>
       <c r="AB3">
-        <v>1.53136690647482</v>
+        <v>1.589913317572892</v>
       </c>
       <c r="AC3">
-        <v>0.6839568345323741</v>
+        <v>0.7491725768321513</v>
       </c>
       <c r="AD3">
-        <v>3.237122302158274</v>
+        <v>3.545784081954295</v>
       </c>
       <c r="AE3">
-        <v>0.03884892086330935</v>
+        <v>0.0425531914893617</v>
       </c>
       <c r="AF3">
-        <v>1.286968244316547</v>
+        <v>1.124142927265563</v>
       </c>
       <c r="AG3">
-        <v>0.1137122302158273</v>
+        <v>0.1245547675334909</v>
       </c>
       <c r="AH3">
-        <v>0.006474820143884892</v>
+        <v>0.007092198581560284</v>
       </c>
       <c r="AI3">
-        <v>3.447913669064748</v>
+        <v>3.776674546887313</v>
       </c>
       <c r="AJ3">
-        <v>0.5503597122302158</v>
+        <v>0.6028368794326241</v>
       </c>
       <c r="AK3">
-        <v>0.3364748201438849</v>
+        <v>0.3685579196217494</v>
       </c>
       <c r="AL3">
-        <v>0.146205035971223</v>
+        <v>0.1601457840819543</v>
       </c>
       <c r="AM3">
-        <v>0.1460431654676259</v>
+        <v>0.1599684791174153</v>
       </c>
       <c r="AN3">
-        <v>0.8902877697841727</v>
+        <v>0.975177304964539</v>
       </c>
       <c r="AO3">
-        <v>0.1503597122302158</v>
+        <v>0.1646966115051221</v>
       </c>
       <c r="AP3">
-        <v>1.881798561151079</v>
+        <v>2.061229314420804</v>
       </c>
       <c r="AQ3">
-        <v>0.1330935251798561</v>
+        <v>0.1379038613081166</v>
       </c>
       <c r="AR3">
-        <v>0.963402131438849</v>
+        <v>0.8490640630417653</v>
       </c>
       <c r="AS3">
-        <v>0.2056951320863309</v>
+        <v>0.1533718088258472</v>
       </c>
       <c r="AT3">
-        <v>0.1782610719424461</v>
+        <v>0.1952583845547675</v>
       </c>
       <c r="AU3">
-        <v>0.2497841726618705</v>
+        <v>0.2736012608353034</v>
       </c>
       <c r="AV3">
-        <v>1.108250782661871</v>
+        <v>1.007662577462569</v>
       </c>
       <c r="AW3">
-        <v>0.3415162313669065</v>
+        <v>0.3386190398739165</v>
       </c>
       <c r="AX3">
-        <v>0.092</v>
+        <v>0.1007722616233254</v>
       </c>
       <c r="AY3">
-        <v>0.06676978417266187</v>
+        <v>0.07313632781717887</v>
       </c>
       <c r="AZ3">
-        <v>0.0683453237410072</v>
+        <v>0.07486209613869188</v>
       </c>
       <c r="BA3">
-        <v>0.1</v>
+        <v>0.1095350669818755</v>
       </c>
       <c r="BB3">
-        <v>0.1010791366906475</v>
+        <v>0.1107171000788022</v>
       </c>
       <c r="BC3">
-        <v>0.001438848920863309</v>
+        <v>0.001576044129235619</v>
       </c>
       <c r="BD3">
-        <v>0.223021582733813</v>
+        <v>0.2442868400315209</v>
       </c>
       <c r="BE3">
-        <v>0.07913669064748201</v>
+        <v>0.08668242710795902</v>
       </c>
       <c r="BF3">
         <v>0</v>
@@ -1114,172 +1114,172 @@
         <v>60</v>
       </c>
       <c r="B4">
-        <v>5.431903282396297</v>
+        <v>5.430753289239733</v>
       </c>
       <c r="C4">
-        <v>169.1877493939813</v>
+        <v>172.2104111356757</v>
       </c>
       <c r="D4">
-        <v>173.6986351574478</v>
+        <v>176.7289916310277</v>
       </c>
       <c r="E4">
-        <v>262.58747805027</v>
+        <v>265.9006960655318</v>
       </c>
       <c r="F4">
-        <v>540.7758774441767</v>
+        <v>502.9354187947058</v>
       </c>
       <c r="G4">
-        <v>52.16760322197145</v>
+        <v>52.99942205420455</v>
       </c>
       <c r="H4">
-        <v>13.3406361212285</v>
+        <v>12.93810686313891</v>
       </c>
       <c r="I4">
-        <v>14.09229099443488</v>
+        <v>14.43346693300467</v>
       </c>
       <c r="J4">
-        <v>5.998028181486877</v>
+        <v>5.287464501756308</v>
       </c>
       <c r="K4">
-        <v>7.03014719956617</v>
+        <v>6.754250447766093</v>
       </c>
       <c r="L4">
-        <v>3.542116910970355</v>
+        <v>3.697799905897668</v>
       </c>
       <c r="M4">
-        <v>5.473866290229083</v>
+        <v>5.69952924215833</v>
       </c>
       <c r="N4">
-        <v>2.732375015446707</v>
+        <v>2.840631030449631</v>
       </c>
       <c r="O4">
-        <v>20.81456603418074</v>
+        <v>21.58336133597242</v>
       </c>
       <c r="P4">
-        <v>2.859138002571895</v>
+        <v>2.984730810999506</v>
       </c>
       <c r="Q4">
-        <v>5.237710182681127</v>
+        <v>5.243466376814968</v>
       </c>
       <c r="R4">
-        <v>3.632715746445505</v>
+        <v>3.792461522792751</v>
       </c>
       <c r="S4">
-        <v>8.37784974579076</v>
+        <v>8.241942753428274</v>
       </c>
       <c r="T4">
-        <v>4.868252896536655</v>
+        <v>5.093805744266537</v>
       </c>
       <c r="U4">
-        <v>0.6375922521670045</v>
+        <v>0.6672454311834292</v>
       </c>
       <c r="V4">
-        <v>10.69904206874055</v>
+        <v>11.18125800714043</v>
       </c>
       <c r="W4">
-        <v>16.41068038296234</v>
+        <v>16.48406269562457</v>
       </c>
       <c r="X4">
-        <v>22.92972514475662</v>
+        <v>22.78300302513044</v>
       </c>
       <c r="Y4">
-        <v>9.291389539472128</v>
+        <v>9.169522313736033</v>
       </c>
       <c r="Z4">
-        <v>8.036790095396755</v>
+        <v>7.929484486384751</v>
       </c>
       <c r="AA4">
-        <v>15.92791845294328</v>
+        <v>16.57990182793024</v>
       </c>
       <c r="AB4">
-        <v>6.220221662084851</v>
+        <v>6.414745206555939</v>
       </c>
       <c r="AC4">
-        <v>4.821561263189952</v>
+        <v>5.041524075995074</v>
       </c>
       <c r="AD4">
-        <v>13.32222006680703</v>
+        <v>13.90404858274003</v>
       </c>
       <c r="AE4">
-        <v>0.4090429912164888</v>
+        <v>0.4279307261182981</v>
       </c>
       <c r="AF4">
-        <v>5.458712152055919</v>
+        <v>5.25364391211117</v>
       </c>
       <c r="AG4">
-        <v>0.7977552401886467</v>
+        <v>0.834141577602706</v>
       </c>
       <c r="AH4">
-        <v>0.1952306173886432</v>
+        <v>0.204322706292276</v>
       </c>
       <c r="AI4">
-        <v>12.83469831687764</v>
+        <v>13.38679694571391</v>
       </c>
       <c r="AJ4">
-        <v>3.282200487980483</v>
+        <v>3.430624947347729</v>
       </c>
       <c r="AK4">
-        <v>4.067162988863774</v>
+        <v>4.255408088259993</v>
       </c>
       <c r="AL4">
-        <v>2.254861336037147</v>
+        <v>2.359522955787477</v>
       </c>
       <c r="AM4">
-        <v>2.263644054215008</v>
+        <v>2.368718057430808</v>
       </c>
       <c r="AN4">
-        <v>7.34182956763585</v>
+        <v>7.678756598970639</v>
       </c>
       <c r="AO4">
-        <v>2.450308868167382</v>
+        <v>2.56409606879239</v>
       </c>
       <c r="AP4">
-        <v>10.64328034438949</v>
+        <v>11.12290715019279</v>
       </c>
       <c r="AQ4">
-        <v>2.053352050203425</v>
+        <v>2.14366994645412</v>
       </c>
       <c r="AR4">
-        <v>4.288062978649821</v>
+        <v>4.041652497877855</v>
       </c>
       <c r="AS4">
-        <v>1.807073019743419</v>
+        <v>1.509991139991264</v>
       </c>
       <c r="AT4">
-        <v>2.74732711424564</v>
+        <v>2.874846213071987</v>
       </c>
       <c r="AU4">
-        <v>3.795730515693905</v>
+        <v>3.971889160505682</v>
       </c>
       <c r="AV4">
-        <v>4.692894163695687</v>
+        <v>4.495458317642192</v>
       </c>
       <c r="AW4">
-        <v>3.08089207406406</v>
+        <v>3.098775666522288</v>
       </c>
       <c r="AX4">
-        <v>1.807563311751408</v>
+        <v>1.891608824712009</v>
       </c>
       <c r="AY4">
-        <v>0.8968386988673681</v>
+        <v>0.9384063935607984</v>
       </c>
       <c r="AZ4">
-        <v>1.823474478878782</v>
+        <v>1.908367780967372</v>
       </c>
       <c r="BA4">
-        <v>2.17272509564667</v>
+        <v>2.273800620802517</v>
       </c>
       <c r="BB4">
-        <v>1.974650069025035</v>
+        <v>2.06646161398685</v>
       </c>
       <c r="BC4">
-        <v>0.05364417807858241</v>
+        <v>0.05614346140443382</v>
       </c>
       <c r="BD4">
-        <v>3.3545970424223</v>
+        <v>3.510267845432892</v>
       </c>
       <c r="BE4">
-        <v>1.702345598184398</v>
+        <v>1.781535361340087</v>
       </c>
       <c r="BF4">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>581</v>
       </c>
       <c r="F5">
-        <v>136</v>
+        <v>140.5</v>
       </c>
       <c r="G5">
         <v>16</v>
@@ -1475,22 +1475,22 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>427.25</v>
+        <v>426</v>
       </c>
       <c r="D6">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E6">
-        <v>798</v>
+        <v>792.2</v>
       </c>
       <c r="F6">
-        <v>1208.5</v>
+        <v>1304.75</v>
       </c>
       <c r="G6">
-        <v>62.12</v>
+        <v>61.18</v>
       </c>
       <c r="H6">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1654,22 +1654,22 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>668.3499999999999</v>
+        <v>668.4</v>
       </c>
       <c r="D7">
         <v>732</v>
       </c>
       <c r="E7">
-        <v>1146.5</v>
+        <v>1145</v>
       </c>
       <c r="F7">
-        <v>1516.5</v>
+        <v>1581.5</v>
       </c>
       <c r="G7">
-        <v>88.90000000000001</v>
+        <v>88.7</v>
       </c>
       <c r="H7">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>9.57845</v>
+        <v>9.4</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1833,25 +1833,25 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="D8">
-        <v>795</v>
+        <v>796.8499999999999</v>
       </c>
       <c r="E8">
-        <v>1258</v>
+        <v>1267.5</v>
       </c>
       <c r="F8">
-        <v>1780</v>
+        <v>1797.625</v>
       </c>
       <c r="G8">
-        <v>107.3</v>
+        <v>108.4</v>
       </c>
       <c r="H8">
-        <v>15</v>
+        <v>14.625</v>
       </c>
       <c r="I8">
-        <v>11.133527775</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1869,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>7.4875</v>
+        <v>3</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1893,13 +1893,13 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>24</v>
+        <v>24.75</v>
       </c>
       <c r="X8">
         <v>30</v>
       </c>
       <c r="Y8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <v>10</v>
@@ -2138,7 +2138,7 @@
         <v>42</v>
       </c>
       <c r="AS9">
-        <v>20</v>
+        <v>19.2</v>
       </c>
       <c r="AT9">
         <v>55</v>

</xml_diff>

<commit_message>
update: update bmgs data
</commit_message>
<xml_diff>
--- a/ALL/ALL_data_grouped_processed_des.xlsx
+++ b/ALL/ALL_data_grouped_processed_des.xlsx
@@ -754,172 +754,172 @@
         <v>815</v>
       </c>
       <c r="F2" t="n">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="G2" t="n">
         <v>399</v>
       </c>
       <c r="H2" t="n">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="I2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="J2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="K2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="L2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="M2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="N2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="O2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="P2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="Q2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="R2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="S2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="T2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="U2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="V2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="W2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="X2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="Y2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="Z2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AA2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AB2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AC2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AD2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AE2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AF2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AG2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AH2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AI2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AK2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AL2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AM2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AN2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AO2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AP2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AR2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AS2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AT2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AU2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AV2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AW2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AX2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AY2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BA2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BB2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BC2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BD2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BE2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BF2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BG2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BH2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
       <c r="BI2" t="n">
-        <v>1276</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="3">
@@ -932,169 +932,169 @@
         <v>5.44295566502463</v>
       </c>
       <c r="C3" t="n">
-        <v>625.9098823082765</v>
+        <v>625.9098861047836</v>
       </c>
       <c r="D3" t="n">
-        <v>677.0424491869919</v>
+        <v>677.0424634146341</v>
       </c>
       <c r="E3" t="n">
-        <v>1076.76145398773</v>
+        <v>1076.764257668712</v>
       </c>
       <c r="F3" t="n">
-        <v>1547.051380368098</v>
+        <v>1548.690778443114</v>
       </c>
       <c r="G3" t="n">
-        <v>94.64789807852965</v>
+        <v>94.64796992481202</v>
       </c>
       <c r="H3" t="n">
-        <v>10.65647858796296</v>
+        <v>9.976722972972972</v>
       </c>
       <c r="I3" t="n">
-        <v>7.663625417894462</v>
+        <v>7.675436137071651</v>
       </c>
       <c r="J3" t="n">
-        <v>1.748324601724138</v>
+        <v>1.737461059190031</v>
       </c>
       <c r="K3" t="n">
-        <v>2.517343341065831</v>
+        <v>2.501658878504673</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8923385579937303</v>
+        <v>0.8867757009345796</v>
       </c>
       <c r="M3" t="n">
-        <v>1.958450705329154</v>
+        <v>1.946246105919003</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7853983556426333</v>
+        <v>0.7805062305295951</v>
       </c>
       <c r="O3" t="n">
-        <v>10.09604183855799</v>
+        <v>10.05654205607476</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7236565755485893</v>
+        <v>0.719158878504673</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.711847440595611</v>
+        <v>1.701191588785047</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8155193792319749</v>
+        <v>0.8104361370716511</v>
       </c>
       <c r="S3" t="n">
-        <v>3.356149114106584</v>
+        <v>3.335303738317758</v>
       </c>
       <c r="T3" t="n">
-        <v>0.4072884012539185</v>
+        <v>0.4047507788161994</v>
       </c>
       <c r="U3" t="n">
-        <v>0.03374608150470219</v>
+        <v>0.03353582554517134</v>
       </c>
       <c r="V3" t="n">
-        <v>2.055956112852665</v>
+        <v>2.043146417445483</v>
       </c>
       <c r="W3" t="n">
-        <v>14.37032843069488</v>
+        <v>14.49653426791278</v>
       </c>
       <c r="X3" t="n">
-        <v>15.61777621841693</v>
+        <v>16.01971183800623</v>
       </c>
       <c r="Y3" t="n">
-        <v>4.044540801175549</v>
+        <v>4.019369158878505</v>
       </c>
       <c r="Z3" t="n">
-        <v>5.989543348354232</v>
+        <v>6.014563862928348</v>
       </c>
       <c r="AA3" t="n">
-        <v>5.850423197492163</v>
+        <v>5.813971962616822</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.581191222570533</v>
+        <v>1.571339563862928</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.7450626959247649</v>
+        <v>0.7404205607476636</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.526332288401254</v>
+        <v>3.504361370716511</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.04231974921630094</v>
+        <v>0.04205607476635514</v>
       </c>
       <c r="AF3" t="n">
-        <v>1.117975998981191</v>
+        <v>1.111020249221184</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.123871473354232</v>
+        <v>0.1230996884735202</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.007053291536050157</v>
+        <v>0.007009345794392523</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.755956112852664</v>
+        <v>3.732554517133956</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.5995297805642633</v>
+        <v>0.5957943925233645</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.3665360501567398</v>
+        <v>0.3642523364485981</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.1592672413793103</v>
+        <v>0.1582788161993769</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.1590909090909091</v>
+        <v>0.1580996884735202</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.9698275862068966</v>
+        <v>0.9637850467289719</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.1637931034482759</v>
+        <v>0.1627725856697819</v>
       </c>
       <c r="AP3" t="n">
-        <v>2.049921630094044</v>
+        <v>2.03714953271028</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.1371473354231975</v>
+        <v>0.1362928348909657</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.8444061880877745</v>
+        <v>0.839151090342679</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.1525304274294671</v>
+        <v>0.1515809968847352</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.1941872178683386</v>
+        <v>0.1929828660436137</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.2721003134796238</v>
+        <v>0.270404984423676</v>
       </c>
       <c r="AV3" t="n">
-        <v>1.002134647962382</v>
+        <v>0.995880062305296</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.3367614119122257</v>
+        <v>0.3393380062305296</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.1002194357366771</v>
+        <v>0.09959501557632398</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.07273510971786833</v>
+        <v>0.07228193146417446</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.07445141065830721</v>
+        <v>0.07398753894080996</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.1089341692789969</v>
+        <v>0.1082554517133956</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.1101097178683386</v>
+        <v>0.1094236760124611</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.001567398119122257</v>
+        <v>0.001557632398753894</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.2429467084639498</v>
+        <v>0.2414330218068536</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08566978193146417</v>
       </c>
       <c r="BF3" t="n">
         <v>0</v>
@@ -1103,10 +1103,10 @@
         <v>0</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.2573824451410658</v>
+        <v>0.01129283489096573</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.8393416927899686</v>
+        <v>0.8403426791277259</v>
       </c>
     </row>
     <row r="4">
@@ -1119,169 +1119,169 @@
         <v>5.416799973795269</v>
       </c>
       <c r="C4" t="n">
-        <v>171.6169442003815</v>
+        <v>171.6169439449899</v>
       </c>
       <c r="D4" t="n">
-        <v>175.9817916165378</v>
+        <v>175.981797166909</v>
       </c>
       <c r="E4" t="n">
-        <v>265.5534544707519</v>
+        <v>265.5547198582155</v>
       </c>
       <c r="F4" t="n">
-        <v>500.5836485157467</v>
+        <v>495.0505359133559</v>
       </c>
       <c r="G4" t="n">
-        <v>52.51453634171216</v>
+        <v>52.5145269745037</v>
       </c>
       <c r="H4" t="n">
-        <v>12.80005776396969</v>
+        <v>12.51796397606443</v>
       </c>
       <c r="I4" t="n">
-        <v>14.40504935775119</v>
+        <v>14.36218134157754</v>
       </c>
       <c r="J4" t="n">
-        <v>5.274529743985168</v>
+        <v>5.259931890642274</v>
       </c>
       <c r="K4" t="n">
-        <v>6.738280218547899</v>
+        <v>6.720174751292573</v>
       </c>
       <c r="L4" t="n">
-        <v>3.688231080096602</v>
+        <v>3.67738093152069</v>
       </c>
       <c r="M4" t="n">
-        <v>5.685724275729099</v>
+        <v>5.670064484618109</v>
       </c>
       <c r="N4" t="n">
-        <v>2.833423469413276</v>
+        <v>2.825258825071417</v>
       </c>
       <c r="O4" t="n">
-        <v>21.53709888552774</v>
+        <v>21.47763890813834</v>
       </c>
       <c r="P4" t="n">
-        <v>2.977011742242182</v>
+        <v>2.96830042245807</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.230599378830392</v>
+        <v>5.216002273481808</v>
       </c>
       <c r="R4" t="n">
-        <v>3.782521873248275</v>
+        <v>3.771255123065122</v>
       </c>
       <c r="S4" t="n">
-        <v>8.223068445491055</v>
+        <v>8.201720138837237</v>
       </c>
       <c r="T4" t="n">
-        <v>5.07989363929634</v>
+        <v>5.064132815135191</v>
       </c>
       <c r="U4" t="n">
-        <v>0.665415980011918</v>
+        <v>0.6633434922714724</v>
       </c>
       <c r="V4" t="n">
-        <v>11.1515684198406</v>
+        <v>11.11792488952686</v>
       </c>
       <c r="W4" t="n">
-        <v>16.47295419333211</v>
+        <v>16.58521717973746</v>
       </c>
       <c r="X4" t="n">
-        <v>22.74163871411715</v>
+        <v>23.05497046131782</v>
       </c>
       <c r="Y4" t="n">
-        <v>9.149252906594466</v>
+        <v>9.126271789740716</v>
       </c>
       <c r="Z4" t="n">
-        <v>7.92019973739828</v>
+        <v>7.901806706384862</v>
       </c>
       <c r="AA4" t="n">
-        <v>16.54003867438572</v>
+        <v>16.49482156729849</v>
       </c>
       <c r="AB4" t="n">
-        <v>6.398190552381331</v>
+        <v>6.379426126646438</v>
       </c>
       <c r="AC4" t="n">
-        <v>5.027970306975853</v>
+        <v>5.012613254485819</v>
       </c>
       <c r="AD4" t="n">
-        <v>13.8683032660278</v>
+        <v>13.8277850285873</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.4267659812804789</v>
+        <v>0.4254464181144004</v>
       </c>
       <c r="AF4" t="n">
-        <v>5.239860740265721</v>
+        <v>5.22427120624288</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.8318995390525159</v>
+        <v>0.829359199733317</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.2037617223884945</v>
+        <v>0.2031262213472014</v>
       </c>
       <c r="AI4" t="n">
-        <v>13.35291478009004</v>
+        <v>13.3145025280377</v>
       </c>
       <c r="AJ4" t="n">
-        <v>3.421484566889841</v>
+        <v>3.411127233352597</v>
       </c>
       <c r="AK4" t="n">
-        <v>4.243797881877596</v>
+        <v>4.230644723870419</v>
       </c>
       <c r="AL4" t="n">
-        <v>2.3530666748669</v>
+        <v>2.345752516447703</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.362236319212684</v>
+        <v>2.35489337517622</v>
       </c>
       <c r="AN4" t="n">
-        <v>7.657987672093526</v>
+        <v>7.634456800255992</v>
       </c>
       <c r="AO4" t="n">
-        <v>2.557076646021944</v>
+        <v>2.549124607830517</v>
       </c>
       <c r="AP4" t="n">
-        <v>11.09337728564644</v>
+        <v>11.05991469889155</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.137801549200824</v>
+        <v>2.131153463473378</v>
       </c>
       <c r="AR4" t="n">
-        <v>4.031030765380454</v>
+        <v>4.019023001713187</v>
       </c>
       <c r="AS4" t="n">
-        <v>1.505883006941647</v>
+        <v>1.501242636902157</v>
       </c>
       <c r="AT4" t="n">
-        <v>2.866979921727244</v>
+        <v>2.858069332321699</v>
       </c>
       <c r="AU4" t="n">
-        <v>3.961022523081721</v>
+        <v>3.948712053549328</v>
       </c>
       <c r="AV4" t="n">
-        <v>4.483719146973247</v>
+        <v>4.470390898140147</v>
       </c>
       <c r="AW4" t="n">
-        <v>3.090358811255201</v>
+        <v>3.082851234817126</v>
       </c>
       <c r="AX4" t="n">
-        <v>1.886423722712931</v>
+        <v>1.880549783918487</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.9358424345621036</v>
+        <v>0.9329377722750313</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1.903129953624377</v>
+        <v>1.89719635288587</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.26756466937121</v>
+        <v>2.26050030884912</v>
       </c>
       <c r="BB4" t="n">
-        <v>2.060797406038949</v>
+        <v>2.054380710595965</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.05598925109558543</v>
+        <v>0.05581455721859475</v>
       </c>
       <c r="BD4" t="n">
-        <v>3.500665093151969</v>
+        <v>3.489786429629616</v>
       </c>
       <c r="BE4" t="n">
-        <v>1.776649687160002</v>
+        <v>1.771114977914812</v>
       </c>
       <c r="BF4" t="n">
         <v>0</v>
@@ -1290,10 +1290,10 @@
         <v>0</v>
       </c>
       <c r="BH4" t="n">
-        <v>3.640204848509379</v>
+        <v>0.1734215168908341</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.367359467084253</v>
+        <v>0.3664306667457159</v>
       </c>
     </row>
     <row r="5">
@@ -1502,13 +1502,13 @@
         <v>794.5</v>
       </c>
       <c r="F6" t="n">
-        <v>1306.75</v>
+        <v>1312.75</v>
       </c>
       <c r="G6" t="n">
         <v>61.745</v>
       </c>
       <c r="H6" t="n">
-        <v>1.7925</v>
+        <v>1.6225</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1695,7 +1695,7 @@
         <v>88</v>
       </c>
       <c r="H7" t="n">
-        <v>5.57</v>
+        <v>5.52</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1876,13 +1876,13 @@
         <v>1267.5</v>
       </c>
       <c r="F8" t="n">
-        <v>1799.5</v>
+        <v>1797.875</v>
       </c>
       <c r="G8" t="n">
         <v>106.4</v>
       </c>
       <c r="H8" t="n">
-        <v>13.475</v>
+        <v>11</v>
       </c>
       <c r="I8" t="n">
         <v>10</v>
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>2.125</v>
+        <v>3</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1927,10 +1927,10 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>24.925</v>
+        <v>25</v>
       </c>
       <c r="X8" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -2075,7 +2075,7 @@
         <v>100</v>
       </c>
       <c r="J9" t="n">
-        <v>27.2727273</v>
+        <v>27.27</v>
       </c>
       <c r="K9" t="n">
         <v>50</v>
@@ -2093,7 +2093,7 @@
         <v>91</v>
       </c>
       <c r="P9" t="n">
-        <v>23.0769231</v>
+        <v>23.08</v>
       </c>
       <c r="Q9" t="n">
         <v>52</v>
@@ -2102,7 +2102,7 @@
         <v>56</v>
       </c>
       <c r="S9" t="n">
-        <v>64.80000000000001</v>
+        <v>64.8</v>
       </c>
       <c r="T9" t="n">
         <v>77.8</v>
@@ -2189,7 +2189,7 @@
         <v>74.7</v>
       </c>
       <c r="AV9" t="n">
-        <v>42.8571429</v>
+        <v>42.86</v>
       </c>
       <c r="AW9" t="n">
         <v>46</v>
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="BH9" t="n">
-        <v>66.67</v>
+        <v>4</v>
       </c>
       <c r="BI9" t="n">
         <v>1</v>

</xml_diff>